<commit_message>
Swim Lanes for MVP
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MVP - v1.0" sheetId="2" r:id="rId1"/>
+    <sheet name="v2.0+" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="142">
   <si>
     <t>Browser</t>
   </si>
@@ -1366,6 +1367,75 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>Set up tables and relationships</t>
+    </r>
+  </si>
+  <si>
+    <t>o   Group Message Box</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>      List of who in the group had a bad run:</t>
+    </r>
+  </si>
+  <si>
+    <t>o   Option to “Light a Fire” Under members</t>
+  </si>
+  <si>
+    <t>READ Group Performance</t>
+  </si>
+  <si>
+    <t>READ Goal Date?</t>
+  </si>
+  <si>
+    <t>Calculate countdown to goal Date</t>
+  </si>
+  <si>
+    <t>Calculate countup from Start Date</t>
+  </si>
+  <si>
+    <t>logic to compile successes</t>
+  </si>
+  <si>
+    <t>logic to compile failures</t>
+  </si>
+  <si>
+    <t>get random quote from array</t>
+  </si>
+  <si>
+    <t>get random image from array</t>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>  Randomized Quote</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>  Randomized image</t>
     </r>
   </si>
 </sst>
@@ -1440,8 +1510,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1526,7 +1612,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1540,6 +1626,14 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1553,6 +1647,14 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1882,11 +1984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88:A113"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1963,6 +2065,407 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30">
+      <c r="A18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="31">
+      <c r="A28" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="31">
+      <c r="A32" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30">
+      <c r="A34" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="31">
+      <c r="A39" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30">
+      <c r="A40" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16">
+      <c r="A45" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30">
+      <c r="A46" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30">
+      <c r="A51" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="7"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D113"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="34" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16">
+      <c r="A3" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" s="9" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Dashboard getMember function working
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="MVP - v1.0" sheetId="2" r:id="rId1"/>
-    <sheet name="v2.0+" sheetId="1" r:id="rId2"/>
+    <sheet name="Current" sheetId="3" r:id="rId1"/>
+    <sheet name="MVP - v1.0" sheetId="2" r:id="rId2"/>
+    <sheet name="v2.0+" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="151">
   <si>
     <t>Browser</t>
   </si>
@@ -1469,6 +1470,77 @@
   </si>
   <si>
     <t>· http GET</t>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Log-in Button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>If logged in, this would be a Log-out button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>  Dashboard Link</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>   STRETCH - Rotate Welcome messages</t>
+    </r>
+  </si>
+  <si>
+    <t>STRETCH - Vertical Centering</t>
   </si>
 </sst>
 </file>
@@ -1542,8 +1614,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1644,7 +1724,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1666,6 +1746,10 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1687,6 +1771,10 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2016,11 +2104,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2061,12 +2149,16 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="6" customHeight="1"/>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" ht="16">
       <c r="A7" s="9" t="s">
         <v>47</v>
@@ -2079,139 +2171,148 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="10" t="s">
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="12" t="s">
-        <v>12</v>
+      <c r="A12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16">
+      <c r="A19" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16">
-      <c r="A15" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16">
-      <c r="A20" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="13" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16">
       <c r="A24" s="14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>83</v>
@@ -2220,135 +2321,121 @@
         <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16">
-      <c r="A25" s="14" t="s">
-        <v>66</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>135</v>
+      <c r="A27" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="12" t="s">
-        <v>129</v>
+      <c r="A28" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16">
-      <c r="A31" s="14" t="s">
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="14" t="s">
         <v>69</v>
       </c>
+      <c r="B30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="B31" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="16" t="s">
+      <c r="A32" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16">
-      <c r="A34" s="14" t="s">
+    <row r="33" spans="1:2" ht="16">
+      <c r="A33" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>137</v>
       </c>
     </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="15" t="s">
-        <v>131</v>
+      <c r="A35" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="12" t="s">
-        <v>27</v>
+      <c r="A36" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>139</v>
+      <c r="A38" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="13" t="s">
+      <c r="A39" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="6" customHeight="1">
-      <c r="A41" s="7"/>
+    <row r="40" spans="1:2" ht="15" customHeight="1">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="2" t="s">
+      <c r="A42" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2365,11 +2452,372 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD14"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="76.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16">
+      <c r="A3" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16">
+      <c r="A22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16">
+      <c r="A26" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16">
+      <c r="A27" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1">
+      <c r="A42" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2531,107 +2979,100 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" ht="60">
+    <row r="26" spans="1:4" ht="16">
+      <c r="A26" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="60">
+      <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="12" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="12" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16">
-      <c r="A31" s="14" t="s">
+    <row r="32" spans="1:4" ht="16">
+      <c r="A32" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="15" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="16" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="15" t="s">
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="16" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31">
-      <c r="A36" s="14" t="s">
+    <row r="37" spans="1:4" ht="31">
+      <c r="A37" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16">
-      <c r="A37" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>83</v>
@@ -2640,420 +3081,434 @@
         <v>9</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16">
+      <c r="A38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="15" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16">
-      <c r="A41" s="17" t="s">
+    <row r="42" spans="1:4" ht="16">
+      <c r="A42" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30">
+      <c r="A44" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" s="12" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="31">
-      <c r="A47" s="14" t="s">
+    <row r="48" spans="1:4" ht="31">
+      <c r="A48" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="15" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="30">
-      <c r="A49" s="15" t="s">
+    <row r="50" spans="1:1" ht="30">
+      <c r="A50" s="15" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="16">
-      <c r="A53" s="14" t="s">
+    <row r="54" spans="1:1" ht="16">
+      <c r="A54" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="30">
-      <c r="A54" s="15" t="s">
+    <row r="55" spans="1:1" ht="30">
+      <c r="A55" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="16" t="s">
+    <row r="56" spans="1:1">
+      <c r="A56" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="30">
-      <c r="A56" s="15" t="s">
+    <row r="57" spans="1:1" ht="30">
+      <c r="A57" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="16">
-      <c r="A57" s="14" t="s">
+    <row r="58" spans="1:1" ht="16">
+      <c r="A58" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="30">
-      <c r="A58" s="15" t="s">
+    <row r="59" spans="1:1" ht="30">
+      <c r="A59" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="46">
-      <c r="A59" s="14" t="s">
+    <row r="60" spans="1:1" ht="46">
+      <c r="A60" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="30">
-      <c r="A60" s="15" t="s">
+    <row r="61" spans="1:1" ht="30">
+      <c r="A61" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="45">
-      <c r="A61" s="15" t="s">
+    <row r="62" spans="1:1" ht="45">
+      <c r="A62" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="30">
-      <c r="A62" s="15" t="s">
+    <row r="63" spans="1:1" ht="30">
+      <c r="A63" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="12" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" s="12" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="31">
-      <c r="A66" s="14" t="s">
+    <row r="67" spans="1:1" ht="31">
+      <c r="A67" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="30">
-      <c r="A67" s="15" t="s">
+    <row r="68" spans="1:1" ht="30">
+      <c r="A68" s="15" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="16" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="31">
-      <c r="A72" s="14" t="s">
+    <row r="73" spans="1:1" ht="31">
+      <c r="A73" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="30">
-      <c r="A73" s="15" t="s">
+    <row r="74" spans="1:1" ht="30">
+      <c r="A74" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="45">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:1" ht="45">
+      <c r="A75" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="12" t="s">
+    <row r="76" spans="1:1">
+      <c r="A76" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="13" t="s">
+    <row r="77" spans="1:1">
+      <c r="A77" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="16">
-      <c r="A77" s="14" t="s">
+    <row r="78" spans="1:1" ht="16">
+      <c r="A78" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="13" t="s">
+    <row r="79" spans="1:1">
+      <c r="A79" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="16">
-      <c r="A79" s="14" t="s">
+    <row r="80" spans="1:1" ht="16">
+      <c r="A80" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="30">
-      <c r="A80" s="13" t="s">
+    <row r="81" spans="1:1" ht="30">
+      <c r="A81" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="31">
-      <c r="A81" s="14" t="s">
+    <row r="82" spans="1:1" ht="31">
+      <c r="A82" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="12" t="s">
+    <row r="83" spans="1:1">
+      <c r="A83" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="30">
-      <c r="A83" s="13" t="s">
+    <row r="84" spans="1:1" ht="30">
+      <c r="A84" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="31">
-      <c r="A84" s="14" t="s">
+    <row r="85" spans="1:1" ht="31">
+      <c r="A85" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="12" t="s">
+    <row r="86" spans="1:1">
+      <c r="A86" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="13" t="s">
+    <row r="87" spans="1:1">
+      <c r="A87" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:1">
+      <c r="A89" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:1">
+      <c r="A90" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:1">
+      <c r="A91" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="3" t="s">
+    <row r="93" spans="1:1">
+      <c r="A93" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:1">
+      <c r="A94" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="3" t="s">
+    <row r="95" spans="1:1">
+      <c r="A95" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:1">
+      <c r="A96" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:1">
+      <c r="A97" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="7"/>
-    </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:1">
+      <c r="A100" s="2" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:1">
+      <c r="A103" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="7"/>
-    </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="7"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:1">
+      <c r="A108" s="2" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:1">
+      <c r="A111" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="7"/>
-    </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="7"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:1">
+      <c r="A114" s="2" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dashboard Personal Stats Box Step/Undo buttons functional
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
     <sheet name="MVP - v1.0" sheetId="2" r:id="rId2"/>
     <sheet name="v2.0+" sheetId="1" r:id="rId3"/>
+    <sheet name="Clean-up" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="154">
   <si>
     <t>Browser</t>
   </si>
@@ -1541,6 +1542,15 @@
   </si>
   <si>
     <t>STRETCH - Vertical Centering</t>
+  </si>
+  <si>
+    <t>Check commenting throughout</t>
+  </si>
+  <si>
+    <t>Check DRYness</t>
+  </si>
+  <si>
+    <t>check if verboses on console.logs</t>
   </si>
 </sst>
 </file>
@@ -1614,8 +1624,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1724,7 +1736,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1750,6 +1762,7 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1775,6 +1788,7 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2104,11 +2118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2177,142 +2191,118 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
+    <row r="10" spans="1:4">
+      <c r="A10" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="12" t="s">
-        <v>12</v>
+      <c r="A11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="13" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="16" t="s">
-        <v>90</v>
+      <c r="D17" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16">
+      <c r="A18" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16">
-      <c r="A19" s="14" t="s">
-        <v>58</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="12" t="s">
-        <v>15</v>
+      <c r="A20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
+      <c r="A21" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16">
-      <c r="A23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16">
       <c r="A24" s="14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>83</v>
@@ -2321,124 +2311,80 @@
         <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="12" t="s">
-        <v>129</v>
+      <c r="A26" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16">
+      <c r="A27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="13" t="s">
-        <v>55</v>
+      <c r="A28" s="15" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16">
-      <c r="A30" s="14" t="s">
-        <v>69</v>
+      <c r="A29" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="15" t="s">
-        <v>25</v>
+      <c r="A31" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="16">
-      <c r="A33" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="12" t="s">
+      <c r="A32" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="13" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1">
-      <c r="A40" s="7"/>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="2" t="s">
         <v>128</v>
       </c>
     </row>
+    <row r="39" spans="1:1" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2815,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
@@ -3521,4 +3467,39 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dashboard Alternate messages for Guest - Swim Lanes update
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="154">
   <si>
     <t>Browser</t>
   </si>
@@ -1516,19 +1516,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">     o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  Dashboard Link</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">    o</t>
     </r>
     <r>
@@ -1551,6 +1538,9 @@
   </si>
   <si>
     <t>check if verboses on console.logs</t>
+  </si>
+  <si>
+    <t>Logic to change links based on current page</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1614,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1736,7 +1728,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1763,6 +1755,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1789,6 +1782,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2118,11 +2112,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2198,52 +2192,58 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>83</v>
@@ -2252,139 +2252,125 @@
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16">
-      <c r="A18" s="14" t="s">
-        <v>66</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>135</v>
+      <c r="A20" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="12" t="s">
-        <v>129</v>
+      <c r="A21" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16">
-      <c r="A24" s="14" t="s">
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" s="14" t="s">
         <v>69</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="B24" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="16" t="s">
+      <c r="A25" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16">
-      <c r="A27" s="14" t="s">
+    <row r="26" spans="1:4" ht="16">
+      <c r="A26" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>137</v>
       </c>
     </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="15" t="s">
-        <v>131</v>
+      <c r="A28" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="12" t="s">
-        <v>27</v>
+      <c r="A29" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>139</v>
+      <c r="A31" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="12" t="s">
-        <v>28</v>
+      <c r="A32" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="A33" s="7"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="7"/>
+      <c r="A34" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2" t="s">
+      <c r="A35" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15" customHeight="1"/>
+    <row r="38" spans="1:1" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2398,11 +2384,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:D7"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2444,81 +2430,111 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="9" t="s">
+      <c r="A5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="10" t="s">
-        <v>48</v>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
-        <v>50</v>
+      <c r="A11" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>10</v>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="12" t="s">
-        <v>12</v>
+      <c r="A14" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
+      <c r="A15" s="15" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
-        <v>56</v>
+      <c r="A16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>83</v>
@@ -2527,53 +2543,44 @@
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>85</v>
+      <c r="A18" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="16" t="s">
-        <v>87</v>
+      <c r="A19" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="16" t="s">
-        <v>90</v>
+      <c r="A20" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16">
+      <c r="A21" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
       <c r="A22" s="14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>83</v>
@@ -2582,167 +2589,121 @@
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="12" t="s">
-        <v>15</v>
+      <c r="A23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="13" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16">
-      <c r="A26" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="28" spans="1:4" ht="16">
+      <c r="A28" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16">
-      <c r="A27" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="13" t="s">
-        <v>55</v>
+      <c r="A30" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16">
-      <c r="A33" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="15" t="s">
-        <v>25</v>
+      <c r="A32" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16">
-      <c r="A36" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="13" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="12" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1">
-      <c r="A42" s="13" t="s">
+    <row r="37" spans="1:2" ht="15" customHeight="1">
+      <c r="A37" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="7"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2762,14 +2723,14 @@
   <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48.83203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="34" style="5" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="5"/>
@@ -2892,6 +2853,9 @@
       <c r="A21" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="B21" s="5" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
@@ -2927,12 +2891,12 @@
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60">
@@ -3481,17 +3445,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Group Stats Box - Install and source UI-Grid dependecies
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="156">
   <si>
     <t>Browser</t>
   </si>
@@ -97,9 +97,6 @@
     <t>o   DB Read</t>
   </si>
   <si>
-    <t>o   STRETCH – Change time from two weeks to:</t>
-  </si>
-  <si>
     <t>o   If true, then countdown to Goal Date</t>
   </si>
   <si>
@@ -575,19 +572,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>  Month</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  One week</t>
     </r>
   </si>
   <si>
@@ -1554,6 +1538,35 @@
   </si>
   <si>
     <t>Logic to change links based on current page</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>      Graph of group performance over last week</t>
+    </r>
+  </si>
+  <si>
+    <t>o   STRETCH – Change time from one week to:</t>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>  Two weeks</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2129,11 +2142,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2161,22 +2174,22 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
@@ -2184,148 +2197,145 @@
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="13" t="s">
+      <c r="D10" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="5" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="13" t="s">
-        <v>56</v>
+      <c r="A19" s="16" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
       <c r="A20" s="14" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16">
-      <c r="A23" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="5" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="15" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2335,34 +2345,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7"/>
-    </row>
-    <row r="33" ht="15" customHeight="1"/>
+      <c r="A27" s="7"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2380,7 +2369,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2408,32 +2397,32 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2441,22 +2430,22 @@
     </row>
     <row r="9" spans="1:4" ht="16">
       <c r="A9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
       <c r="A10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -2464,10 +2453,10 @@
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -2483,7 +2472,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>6</v>
@@ -2491,76 +2480,76 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
       <c r="A22" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2570,7 +2559,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>6</v>
@@ -2578,137 +2567,137 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="14" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
       <c r="A27" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2716,12 +2705,12 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2739,9 +2728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2769,57 +2758,57 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2827,7 +2816,7 @@
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>5</v>
@@ -2835,7 +2824,7 @@
     </row>
     <row r="14" spans="1:4" ht="16">
       <c r="A14" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>6</v>
@@ -2843,45 +2832,45 @@
     </row>
     <row r="15" spans="1:4" ht="16">
       <c r="A15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16">
       <c r="A18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
       <c r="A20" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16">
       <c r="A21" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>6</v>
@@ -2889,12 +2878,12 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>8</v>
@@ -2908,17 +2897,17 @@
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60">
       <c r="A28" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>11</v>
@@ -2931,7 +2920,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>6</v>
@@ -2939,90 +2928,90 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16">
       <c r="A32" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="31">
       <c r="A37" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3030,49 +3019,49 @@
         <v>13</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16">
       <c r="A42" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
@@ -3080,21 +3069,21 @@
         <v>14</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3104,7 +3093,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>6</v>
@@ -3112,12 +3101,12 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="31">
       <c r="A48" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -3127,202 +3116,202 @@
     </row>
     <row r="50" spans="1:1" ht="30">
       <c r="A50" s="15" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="16" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="16">
       <c r="A54" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="30">
       <c r="A55" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="30">
       <c r="A57" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="16">
       <c r="A58" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="30">
       <c r="A59" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="46">
       <c r="A60" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="30">
       <c r="A61" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="45">
       <c r="A62" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="30">
       <c r="A63" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="31">
       <c r="A67" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="30">
       <c r="A68" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="31">
       <c r="A73" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="30">
       <c r="A74" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="45">
       <c r="A75" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="16">
       <c r="A78" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="16">
       <c r="A80" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="30">
       <c r="A81" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="31">
       <c r="A82" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="30">
       <c r="A84" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="31">
       <c r="A85" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:1">
@@ -3332,7 +3321,7 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:1">
@@ -3342,22 +3331,22 @@
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="1:1">
@@ -3365,37 +3354,37 @@
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:1">
@@ -3403,27 +3392,27 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="112" spans="1:1">
@@ -3431,12 +3420,12 @@
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3462,17 +3451,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Group Stats Box - first steps
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="155">
   <si>
     <t>Browser</t>
   </si>
@@ -442,19 +442,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>   STRETCH - Get Current timezone from user</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  DB READ</t>
     </r>
   </si>
   <si>
@@ -1640,8 +1627,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1756,7 +1745,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1785,6 +1774,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1813,6 +1803,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2142,11 +2133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2184,7 +2175,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2207,7 +2198,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -2215,143 +2206,113 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
       <c r="A10" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="D14" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="12" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16">
+      <c r="A17" s="14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16">
-      <c r="A17" s="14" t="s">
-        <v>67</v>
-      </c>
       <c r="B17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16">
-      <c r="A20" s="14" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    <row r="21" spans="1:2">
+      <c r="A21" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2407,22 +2368,22 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2456,7 +2417,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -2472,7 +2433,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>6</v>
@@ -2480,76 +2441,76 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
       <c r="A22" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2559,7 +2520,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>6</v>
@@ -2567,35 +2528,35 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
       <c r="A27" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2603,7 +2564,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2611,36 +2572,36 @@
         <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2648,25 +2609,25 @@
         <v>24</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2676,18 +2637,18 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2697,7 +2658,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2705,12 +2666,12 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2726,11 +2687,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2860,7 +2821,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2897,12 +2858,12 @@
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60">
@@ -2920,7 +2881,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>6</v>
@@ -2928,90 +2889,90 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16">
       <c r="A32" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="31">
       <c r="A37" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3019,49 +2980,49 @@
         <v>13</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16">
       <c r="A42" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
@@ -3069,21 +3030,21 @@
         <v>14</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3093,7 +3054,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>6</v>
@@ -3101,92 +3062,107 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="31">
       <c r="A48" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="30">
+    <row r="50" spans="1:4" ht="30">
       <c r="A50" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="16" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="16" t="s">
+    <row r="53" spans="1:4">
+      <c r="A53" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="16" t="s">
+    <row r="54" spans="1:4" ht="16">
+      <c r="A54" s="14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="16">
-      <c r="A54" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="30">
+      <c r="B54" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30">
       <c r="A55" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="16" t="s">
+      <c r="B55" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16">
+      <c r="A57" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30">
+      <c r="A58" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="46">
+      <c r="A59" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="45">
+      <c r="A61" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30">
+      <c r="A62" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="13" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="30">
-      <c r="A57" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="16">
-      <c r="A58" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="30">
-      <c r="A59" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="46">
-      <c r="A60" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="30">
-      <c r="A61" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="45">
-      <c r="A62" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="30">
-      <c r="A63" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -3194,19 +3170,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="31">
-      <c r="A67" s="14" t="s">
+    <row r="66" spans="1:1" ht="31">
+      <c r="A66" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="30">
+      <c r="A67" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="16" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="30">
-      <c r="A68" s="15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:1">
@@ -3216,149 +3192,149 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="31">
+      <c r="A72" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="31">
-      <c r="A73" s="14" t="s">
+    <row r="73" spans="1:1" ht="30">
+      <c r="A73" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="45">
+      <c r="A74" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="30">
-      <c r="A74" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="45">
-      <c r="A75" s="16" t="s">
+    <row r="75" spans="1:1">
+      <c r="A75" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="13" t="s">
+    <row r="77" spans="1:1" ht="16">
+      <c r="A77" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16">
-      <c r="A78" s="14" t="s">
+    <row r="78" spans="1:1">
+      <c r="A78" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="13" t="s">
+    <row r="79" spans="1:1" ht="16">
+      <c r="A79" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="30">
+      <c r="A80" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="16">
-      <c r="A80" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="30">
-      <c r="A81" s="13" t="s">
+    <row r="81" spans="1:1" ht="31">
+      <c r="A81" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="31">
-      <c r="A82" s="14" t="s">
+    <row r="82" spans="1:1">
+      <c r="A82" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="30">
+      <c r="A83" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="30">
-      <c r="A84" s="13" t="s">
+    <row r="84" spans="1:1" ht="31">
+      <c r="A84" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="31">
-      <c r="A85" s="14" t="s">
+    <row r="85" spans="1:1">
+      <c r="A85" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="13" t="s">
-        <v>80</v>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="3" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:1">
+      <c r="A93" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="7"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="7"/>
-    </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3368,12 +3344,12 @@
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3383,20 +3359,20 @@
       </c>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="7"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="7"/>
-    </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="3" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3406,26 +3382,21 @@
       </c>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="7"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="7"/>
-    </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3451,17 +3422,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Swim Lanes and Moment bug fix
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="156">
   <si>
     <t>Browser</t>
   </si>
@@ -1553,6 +1553,19 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>  Two weeks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>     If click undo "yes" then "X" should disappear from grid</t>
     </r>
   </si>
 </sst>
@@ -2133,11 +2146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2198,121 +2211,104 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="14" t="s">
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="14" t="s">
         <v>66</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="16" t="s">
+      <c r="A15" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16">
-      <c r="A17" s="14" t="s">
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>134</v>
       </c>
     </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="15" t="s">
-        <v>128</v>
+      <c r="A18" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="12" t="s">
-        <v>26</v>
+      <c r="A19" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>136</v>
+      <c r="A21" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="12" t="s">
-        <v>27</v>
+      <c r="A22" s="13" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1"/>
+      <c r="A23" s="7"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Tracking progress in Swim Lanes
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="156">
   <si>
     <t>Browser</t>
   </si>
@@ -1556,17 +1556,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>     If click undo "yes" then "X" should disappear from grid</t>
-    </r>
+    <t>o   STRETCH – change autogridsize to not be time-based:</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1630,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1758,7 +1750,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1788,6 +1780,7 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1817,6 +1810,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2146,11 +2140,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2206,109 +2200,94 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="12" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="12" t="s">
-        <v>126</v>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="13" t="s">
-        <v>53</v>
+      <c r="A11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="13" t="s">
-        <v>54</v>
+      <c r="A12" s="16" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="14" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16">
-      <c r="A16" s="14" t="s">
-        <v>127</v>
+      <c r="A15" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
-        <v>128</v>
+      <c r="A17" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1"/>
+      <c r="A20" s="7"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2683,11 +2662,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57:XFD57"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3091,307 +3070,312 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16">
-      <c r="A54" s="14" t="s">
+    <row r="54" spans="1:4" ht="45">
+      <c r="A54" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16">
+      <c r="A55" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D55" s="5" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30">
+      <c r="A57" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16">
-      <c r="A57" s="14" t="s">
+    <row r="58" spans="1:4" ht="16">
+      <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="15" t="s">
+    <row r="59" spans="1:4" ht="30">
+      <c r="A59" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="46">
-      <c r="A59" s="14" t="s">
+    <row r="60" spans="1:4" ht="46">
+      <c r="A60" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="15" t="s">
+    <row r="61" spans="1:4" ht="30">
+      <c r="A61" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45">
-      <c r="A61" s="15" t="s">
+    <row r="62" spans="1:4" ht="45">
+      <c r="A62" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30">
-      <c r="A62" s="15" t="s">
+    <row r="63" spans="1:4" ht="30">
+      <c r="A63" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="12" t="s">
+    <row r="64" spans="1:4">
+      <c r="A64" s="12" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="31">
-      <c r="A66" s="14" t="s">
+    <row r="67" spans="1:1" ht="31">
+      <c r="A67" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="30">
-      <c r="A67" s="15" t="s">
+    <row r="68" spans="1:1" ht="30">
+      <c r="A68" s="15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="31">
-      <c r="A72" s="14" t="s">
+    <row r="73" spans="1:1" ht="31">
+      <c r="A73" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="30">
-      <c r="A73" s="15" t="s">
+    <row r="74" spans="1:1" ht="30">
+      <c r="A74" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="45">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:1" ht="45">
+      <c r="A75" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="12" t="s">
+    <row r="76" spans="1:1">
+      <c r="A76" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="13" t="s">
+    <row r="77" spans="1:1">
+      <c r="A77" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="16">
-      <c r="A77" s="14" t="s">
+    <row r="78" spans="1:1" ht="16">
+      <c r="A78" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="13" t="s">
+    <row r="79" spans="1:1">
+      <c r="A79" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="16">
-      <c r="A79" s="14" t="s">
+    <row r="80" spans="1:1" ht="16">
+      <c r="A80" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="30">
-      <c r="A80" s="13" t="s">
+    <row r="81" spans="1:1" ht="30">
+      <c r="A81" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="31">
-      <c r="A81" s="14" t="s">
+    <row r="82" spans="1:1" ht="31">
+      <c r="A82" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="12" t="s">
+    <row r="83" spans="1:1">
+      <c r="A83" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="30">
-      <c r="A83" s="13" t="s">
+    <row r="84" spans="1:1" ht="30">
+      <c r="A84" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="31">
-      <c r="A84" s="14" t="s">
+    <row r="85" spans="1:1" ht="31">
+      <c r="A85" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="12" t="s">
+    <row r="86" spans="1:1">
+      <c r="A86" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="13" t="s">
+    <row r="87" spans="1:1">
+      <c r="A87" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:1">
+      <c r="A89" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:1">
+      <c r="A90" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:1">
+      <c r="A91" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="3" t="s">
+    <row r="93" spans="1:1">
+      <c r="A93" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:1">
+      <c r="A94" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="3" t="s">
+    <row r="95" spans="1:1">
+      <c r="A95" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:1">
+      <c r="A96" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:1">
+      <c r="A97" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="7"/>
-    </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:1">
+      <c r="A100" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:1">
+      <c r="A103" s="2" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="7"/>
-    </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="7"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:1">
+      <c r="A108" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:1">
+      <c r="A111" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="7"/>
-    </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="7"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:1">
+      <c r="A114" s="2" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB and query changes for better e-mail security
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
   <si>
     <t>Browser</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>o   STRETCH – change autogridsize to not be time-based:</t>
+  </si>
+  <si>
+    <t>o   STRETCH – change results to not use e-mails as identifiers.</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2147,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2662,11 +2665,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3075,307 +3078,312 @@
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:4" ht="45">
+      <c r="A55" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16">
+      <c r="A56" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
       <c r="A57" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30">
+      <c r="A58" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B58" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16">
-      <c r="A58" s="14" t="s">
+    <row r="59" spans="1:4" ht="16">
+      <c r="A59" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="15" t="s">
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="46">
-      <c r="A60" s="14" t="s">
+    <row r="61" spans="1:4" ht="46">
+      <c r="A61" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30">
-      <c r="A61" s="15" t="s">
+    <row r="62" spans="1:4" ht="30">
+      <c r="A62" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45">
-      <c r="A62" s="15" t="s">
+    <row r="63" spans="1:4" ht="45">
+      <c r="A63" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="15" t="s">
+    <row r="64" spans="1:4" ht="30">
+      <c r="A64" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="12" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" s="12" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="31">
-      <c r="A67" s="14" t="s">
+    <row r="68" spans="1:1" ht="31">
+      <c r="A68" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="30">
-      <c r="A68" s="15" t="s">
+    <row r="69" spans="1:1" ht="30">
+      <c r="A69" s="15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="31">
-      <c r="A73" s="14" t="s">
+    <row r="74" spans="1:1" ht="31">
+      <c r="A74" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="30">
-      <c r="A74" s="15" t="s">
+    <row r="75" spans="1:1" ht="30">
+      <c r="A75" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="45">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:1" ht="45">
+      <c r="A76" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="12" t="s">
+    <row r="77" spans="1:1">
+      <c r="A77" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="13" t="s">
+    <row r="78" spans="1:1">
+      <c r="A78" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16">
-      <c r="A78" s="14" t="s">
+    <row r="79" spans="1:1" ht="16">
+      <c r="A79" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="13" t="s">
+    <row r="80" spans="1:1">
+      <c r="A80" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="16">
-      <c r="A80" s="14" t="s">
+    <row r="81" spans="1:1" ht="16">
+      <c r="A81" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="30">
-      <c r="A81" s="13" t="s">
+    <row r="82" spans="1:1" ht="30">
+      <c r="A82" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="31">
-      <c r="A82" s="14" t="s">
+    <row r="83" spans="1:1" ht="31">
+      <c r="A83" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="12" t="s">
+    <row r="84" spans="1:1">
+      <c r="A84" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="30">
-      <c r="A84" s="13" t="s">
+    <row r="85" spans="1:1" ht="30">
+      <c r="A85" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="31">
-      <c r="A85" s="14" t="s">
+    <row r="86" spans="1:1" ht="31">
+      <c r="A86" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="12" t="s">
+    <row r="87" spans="1:1">
+      <c r="A87" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="13" t="s">
+    <row r="88" spans="1:1">
+      <c r="A88" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:1">
+      <c r="A90" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:1">
+      <c r="A91" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="3" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:1">
+      <c r="A93" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="3" t="s">
+    <row r="94" spans="1:1">
+      <c r="A94" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:1">
+      <c r="A95" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="3" t="s">
+    <row r="96" spans="1:1">
+      <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="4" t="s">
+    <row r="97" spans="1:1">
+      <c r="A97" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:1">
+      <c r="A98" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="7"/>
-    </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="7"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:1">
+      <c r="A101" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:1">
+      <c r="A104" s="2" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="7"/>
-    </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="7"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:1">
+      <c r="A109" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:1">
+      <c r="A112" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="7"/>
-    </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="7"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:1">
+      <c r="A115" s="2" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
join Group functionality for no group members
</commit_message>
<xml_diff>
--- a/Total Mercy Swim Lanes.xlsx
+++ b/Total Mercy Swim Lanes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="157">
   <si>
     <t>Browser</t>
   </si>
@@ -115,9 +115,6 @@
     <t>o   Majority Approval is enough to approve</t>
   </si>
   <si>
-    <t>o   STRETCH - Group Message Box</t>
-  </si>
-  <si>
     <t>o   Option to “Hi-5” Successes</t>
   </si>
   <si>
@@ -624,45 +621,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>      List of who in the group had a successful run:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  Day</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  Week</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>§</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>  Year</t>
     </r>
   </si>
   <si>
@@ -1560,6 +1518,28 @@
   </si>
   <si>
     <t>o   STRETCH – change results to not use e-mails as identifiers.</t>
+  </si>
+  <si>
+    <t>Figure out if no group yet…</t>
+  </si>
+  <si>
+    <t>Prefs page?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>  STRETCH - create a new group if no group</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1633,8 +1613,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1753,7 +1747,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1784,6 +1778,13 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1814,6 +1815,13 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2143,11 +2151,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2175,122 +2183,58 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="9" t="s">
-        <v>46</v>
-      </c>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="12" t="s">
-        <v>126</v>
-      </c>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="13" t="s">
-        <v>53</v>
+      <c r="A8" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>133</v>
-      </c>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>134</v>
-      </c>
+      <c r="A12" s="7"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1"/>
+      <c r="A14" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2336,32 +2280,32 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2369,22 +2313,22 @@
     </row>
     <row r="9" spans="1:4" ht="16">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
       <c r="A10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -2392,10 +2336,10 @@
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -2411,7 +2355,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>6</v>
@@ -2419,76 +2363,76 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
       <c r="A22" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2498,7 +2442,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>6</v>
@@ -2506,35 +2450,35 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
       <c r="A27" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2542,7 +2486,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2550,93 +2494,93 @@
         <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2644,12 +2588,12 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2665,11 +2609,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2697,57 +2641,57 @@
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2755,7 +2699,7 @@
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>5</v>
@@ -2763,7 +2707,7 @@
     </row>
     <row r="14" spans="1:4" ht="16">
       <c r="A14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>6</v>
@@ -2771,45 +2715,45 @@
     </row>
     <row r="15" spans="1:4" ht="16">
       <c r="A15" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
       <c r="A20" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16">
       <c r="A21" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>6</v>
@@ -2817,12 +2761,12 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>8</v>
@@ -2836,17 +2780,17 @@
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60">
       <c r="A28" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>11</v>
@@ -2859,7 +2803,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>6</v>
@@ -2867,90 +2811,90 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16">
       <c r="A32" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="C34" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="31">
       <c r="A37" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2958,49 +2902,49 @@
         <v>13</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16">
       <c r="A42" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="C42" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
@@ -3008,21 +2952,21 @@
         <v>14</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3032,7 +2976,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>6</v>
@@ -3040,12 +2984,12 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="31">
       <c r="A48" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3055,46 +2999,46 @@
     </row>
     <row r="50" spans="1:4" ht="30">
       <c r="A50" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="45">
       <c r="A54" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="45">
       <c r="A55" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="16">
       <c r="A56" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
@@ -3102,7 +3046,7 @@
         <v>17</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
@@ -3110,12 +3054,12 @@
         <v>18</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="16">
       <c r="A59" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30">
@@ -3125,7 +3069,7 @@
     </row>
     <row r="61" spans="1:4" ht="46">
       <c r="A61" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30">
@@ -3143,134 +3087,140 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:2">
       <c r="A65" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="31">
+    <row r="68" spans="1:2" ht="31">
       <c r="A68" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30">
+      <c r="A69" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16">
+      <c r="A70" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="31">
+      <c r="A71" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="30">
-      <c r="A69" s="15" t="s">
+    <row r="72" spans="1:2" ht="30">
+      <c r="A72" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="16" t="s">
+    <row r="73" spans="1:2" ht="45">
+      <c r="A73" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="16" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="16" t="s">
+    <row r="77" spans="1:2" ht="16">
+      <c r="A77" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="31">
-      <c r="A74" s="14" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="30">
-      <c r="A75" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="45">
-      <c r="A76" s="16" t="s">
+    <row r="79" spans="1:2" ht="16">
+      <c r="A79" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="30">
+      <c r="A80" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="12" t="s">
+    <row r="81" spans="1:1" ht="31">
+      <c r="A81" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="16">
-      <c r="A79" s="14" t="s">
+    <row r="83" spans="1:1" ht="30">
+      <c r="A83" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="13" t="s">
+    <row r="84" spans="1:1" ht="31">
+      <c r="A84" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="16">
-      <c r="A81" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="30">
-      <c r="A82" s="13" t="s">
+    <row r="85" spans="1:1">
+      <c r="A85" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="31">
-      <c r="A83" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="30">
-      <c r="A85" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="31">
-      <c r="A86" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="13" t="s">
-        <v>79</v>
+      <c r="A88" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="1" t="s">
-        <v>105</v>
+      <c r="A90" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:1">
@@ -3280,111 +3230,101 @@
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="3" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="7"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="3" t="s">
+    <row r="99" spans="1:1">
+      <c r="A99" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="4" t="s">
+    <row r="100" spans="1:1">
+      <c r="A100" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="2" t="s">
+    <row r="101" spans="1:1">
+      <c r="A101" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="7"/>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="1" t="s">
+    <row r="102" spans="1:1">
+      <c r="A102" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="7"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="2" t="s">
+    <row r="107" spans="1:1">
+      <c r="A107" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="3" t="s">
+    <row r="108" spans="1:1">
+      <c r="A108" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="3" t="s">
+    <row r="109" spans="1:1">
+      <c r="A109" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="7"/>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="1" t="s">
+    <row r="110" spans="1:1">
+      <c r="A110" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109" s="2" t="s">
+    <row r="111" spans="1:1">
+      <c r="A111" s="7"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110" s="3" t="s">
+    <row r="113" spans="1:1">
+      <c r="A113" s="2" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="7"/>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3410,17 +3350,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>